<commit_message>
resolution statistics and folder edits
</commit_message>
<xml_diff>
--- a/Output/Class Statistics/Finalized/test_train_class_cnts.xlsx
+++ b/Output/Class Statistics/Finalized/test_train_class_cnts.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -452,6 +452,16 @@
           <t>Test</t>
         </is>
       </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Percent</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
@@ -465,6 +475,14 @@
       <c r="C2" s="2" t="n">
         <v>279</v>
       </c>
+      <c r="D2" s="2" t="n">
+        <v>1419</v>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>18.94%</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
@@ -478,6 +496,14 @@
       <c r="C3" s="2" t="n">
         <v>189</v>
       </c>
+      <c r="D3" s="2" t="n">
+        <v>902</v>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>12.04%</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
@@ -491,6 +517,14 @@
       <c r="C4" s="2" t="n">
         <v>441</v>
       </c>
+      <c r="D4" s="2" t="n">
+        <v>2057</v>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>27.46%</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
@@ -503,6 +537,14 @@
       </c>
       <c r="C5" s="2" t="n">
         <v>580</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>3114</v>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>41.56%</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated counts and set seed on sample images draw
</commit_message>
<xml_diff>
--- a/Output/Class Statistics/Finalized/test_train_class_cnts.xlsx
+++ b/Output/Class Statistics/Finalized/test_train_class_cnts.xlsx
@@ -428,7 +428,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -547,6 +547,23 @@
         </is>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>6003</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>1489</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>7492</v>
+      </c>
+      <c r="E6" s="2" t="inlineStr"/>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>